<commit_message>
Fix uncertainty bounds in GaAs LCI
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-PV-GaAs.xlsx
+++ b/premise/data/additional_inventories/lci-PV-GaAs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EE2B8-EBB8-4574-A0C7-9B60E5B3901D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BA4066-325E-3C46-A2F7-CE0061120767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV_GaAs" sheetId="3" r:id="rId1"/>
@@ -899,9 +899,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1027,7 +1027,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1392,25 +1392,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" zoomScale="108" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B428" sqref="B428"/>
+    <sheetView tabSelected="1" topLeftCell="B424" zoomScale="108" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="I443" sqref="I443"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>238</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>B5</f>
         <v>coating, drying, optical lithography</v>
@@ -1546,7 +1546,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>259</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>238</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>239</v>
       </c>
@@ -1827,12 +1827,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>B26</f>
         <v>electroplating</v>
@@ -1886,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>99</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>238</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>239</v>
       </c>
@@ -2159,12 +2159,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>7</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>B47</f>
         <v>wet etching</v>
@@ -2218,7 +2218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>238</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>239</v>
       </c>
@@ -2406,12 +2406,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>7</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f>B64</f>
         <v>metal organic vapor phase epitaxy (MOVPE), for GaAs photovoltaic panel</v>
@@ -2465,7 +2465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>273</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>103</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>262</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>107</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>104</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2684,14 +2684,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C84" s="28"/>
       <c r="D84" s="7"/>
       <c r="E84" s="28"/>
       <c r="F84" s="28"/>
       <c r="G84" s="28"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C85" s="28"/>
       <c r="D85" s="7"/>
       <c r="E85" s="28"/>
@@ -2699,7 +2699,7 @@
       <c r="G85" s="28"/>
       <c r="I85" s="28"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>238</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>239</v>
       </c>
@@ -2763,12 +2763,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>7</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
         <f>B86</f>
         <v>epitaxial lift-off (ELO)</v>
@@ -2825,7 +2825,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>74</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>258</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>89</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>238</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>14</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>239</v>
       </c>
@@ -3115,12 +3115,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>7</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
         <f>B107</f>
         <v>polycrystalline GaAs boule production</v>
@@ -3176,7 +3176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>247</v>
       </c>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="I118" s="9"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>248</v>
       </c>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="I119" s="9"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
         <v>123</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
         <v>127</v>
       </c>
@@ -3302,10 +3302,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C123" s="6"/>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>0</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>238</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>2</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>14</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>4</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>239</v>
       </c>
@@ -3369,12 +3369,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>7</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="str">
         <f>B124</f>
         <v>7N gallium production</v>
@@ -3429,7 +3429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
         <v>129</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>120</v>
       </c>
@@ -3481,13 +3481,13 @@
         <v>131</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="9"/>
       <c r="B137" s="9"/>
       <c r="C137" s="6"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>0</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>238</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>14</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>4</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>239</v>
       </c>
@@ -3551,12 +3551,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>7</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>B138</f>
         <v>7N arsenic production</v>
@@ -3611,7 +3611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>107</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>273</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>134</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>120</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>0</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>238</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>14</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>1</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>4</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>239</v>
       </c>
@@ -3779,12 +3779,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>7</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="str">
         <f>B154</f>
         <v>single-crystal GaAs boule production</v>
@@ -3839,7 +3839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="I165" s="9"/>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="9" t="s">
         <v>139</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="9" t="s">
         <v>123</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>120</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
         <v>127</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="9" t="s">
         <v>127</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="9" t="s">
         <v>127</v>
       </c>
@@ -4019,14 +4019,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="11"/>
       <c r="B172" s="11"/>
       <c r="C172" s="11"/>
       <c r="D172" s="12"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>238</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>14</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>1</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>4</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>239</v>
       </c>
@@ -4090,12 +4090,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>7</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="str">
         <f>B173</f>
         <v>GaAs ingot production - x-ray, cropping, grinding notch</v>
@@ -4151,7 +4151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>249</v>
       </c>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="I184" s="9"/>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="9" t="s">
         <v>144</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>251</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>120</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>120</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>120</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="9" t="s">
         <v>127</v>
       </c>
@@ -4328,14 +4328,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="9"/>
       <c r="B191" s="9"/>
       <c r="C191" s="13"/>
       <c r="D191" s="14"/>
       <c r="E191" s="9"/>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>0</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>238</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>14</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>1</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>8</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>4</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>239</v>
       </c>
@@ -4399,12 +4399,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>7</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="str">
         <f>B192</f>
         <v>diamond saw production</v>
@@ -4460,7 +4460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" s="9" t="s">
         <v>151</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>252</v>
       </c>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="I204" s="9"/>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>120</v>
       </c>
@@ -4536,13 +4536,13 @@
         <v>131</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" s="9"/>
       <c r="B206" s="9"/>
       <c r="C206" s="6"/>
       <c r="D206" s="10"/>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>0</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>238</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>2</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>14</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>1</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>8</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>4</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>239</v>
       </c>
@@ -4606,12 +4606,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>7</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" t="str">
         <f>B207</f>
         <v>synthetic diamond production</v>
@@ -4667,7 +4667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="15" t="s">
         <v>204</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>273</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>120</v>
       </c>
@@ -4745,10 +4745,10 @@
         <v>131</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" s="18"/>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>0</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>238</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>2</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>14</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>1</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>8</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>4</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>239</v>
       </c>
@@ -4812,12 +4812,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>7</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" t="str">
         <f>B222</f>
         <v>raw GaAs wafer production</v>
@@ -4873,7 +4873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>250</v>
       </c>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="I233" s="9"/>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" s="9" t="s">
         <v>144</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" s="9" t="s">
         <v>254</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>251</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>120</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>120</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" s="9" t="s">
         <v>127</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
@@ -5061,7 +5061,7 @@
       <c r="H240" s="2"/>
       <c r="I240" s="2"/>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>0</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>238</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>2</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>14</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>1</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>8</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>4</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>239</v>
       </c>
@@ -5125,12 +5125,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>7</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="str">
         <f>B241</f>
         <v>sawing slurry production</v>
@@ -5185,7 +5185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" s="9" t="s">
         <v>156</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" s="9" t="s">
         <v>264</v>
       </c>
@@ -5237,13 +5237,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B254" s="9"/>
       <c r="C254" s="9"/>
       <c r="D254" s="14"/>
       <c r="E254" s="9"/>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>0</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>238</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>2</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>14</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="259" spans="1:9">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>8</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>4</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="262" spans="1:9">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>239</v>
       </c>
@@ -5307,12 +5307,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
         <v>7</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="265" spans="1:9">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" t="str">
         <f>B255</f>
         <v>etched GaAs wafer production - cleaning, etching</v>
@@ -5368,7 +5368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:9">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>253</v>
       </c>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="I266" s="9"/>
     </row>
-    <row r="267" spans="1:9">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" s="9" t="s">
         <v>162</v>
       </c>
@@ -5416,7 +5416,7 @@
       </c>
       <c r="I267" s="9"/>
     </row>
-    <row r="268" spans="1:9">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" s="9" t="s">
         <v>170</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="269" spans="1:9">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="9" t="s">
         <v>110</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="270" spans="1:9">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>120</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="271" spans="1:9">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>120</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="272" spans="1:9">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" s="9" t="s">
         <v>127</v>
       </c>
@@ -5546,14 +5546,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="273" spans="1:9">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" s="9"/>
       <c r="B273" s="9"/>
       <c r="C273" s="13"/>
       <c r="D273" s="14"/>
       <c r="E273" s="9"/>
     </row>
-    <row r="274" spans="1:9">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
         <v>0</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="275" spans="1:9">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>238</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="276" spans="1:9">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>2</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>14</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>1</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="279" spans="1:9">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>8</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:9">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>4</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="281" spans="1:9">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>239</v>
       </c>
@@ -5617,12 +5617,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="282" spans="1:9">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="283" spans="1:9">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>7</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="284" spans="1:9">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" t="str">
         <f>B274</f>
         <v>pre-polished GaAs wafer production</v>
@@ -5678,7 +5678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:9">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>255</v>
       </c>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="I285" s="9"/>
     </row>
-    <row r="286" spans="1:9">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" s="9" t="s">
         <v>113</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="287" spans="1:9">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>254</v>
       </c>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="I287" s="9"/>
     </row>
-    <row r="288" spans="1:9">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>120</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="289" spans="1:9">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A289" s="9" t="s">
         <v>127</v>
       </c>
@@ -5804,14 +5804,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="290" spans="1:9">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A290" s="9"/>
       <c r="B290" s="9"/>
       <c r="C290" s="13"/>
       <c r="D290" s="14"/>
       <c r="E290" s="9"/>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
         <v>0</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>238</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>2</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>14</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>1</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>8</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>4</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>239</v>
       </c>
@@ -5875,12 +5875,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A300" s="2" t="s">
         <v>7</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A301" t="str">
         <f>B291</f>
         <v>double-polished GaAs wafer production - chemical, mechanical polishing (CMP)</v>
@@ -5936,7 +5936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A302" s="9" t="s">
         <v>256</v>
       </c>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="I302" s="9"/>
     </row>
-    <row r="303" spans="1:9">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A303" s="9" t="s">
         <v>113</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="304" spans="1:9">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" s="9" t="s">
         <v>258</v>
       </c>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="I304" s="9"/>
     </row>
-    <row r="305" spans="1:9">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>120</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="306" spans="1:9">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" s="9" t="s">
         <v>127</v>
       </c>
@@ -6062,14 +6062,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="307" spans="1:9">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" s="9"/>
       <c r="B307" s="9"/>
       <c r="C307" s="13"/>
       <c r="D307" s="14"/>
       <c r="E307" s="9"/>
     </row>
-    <row r="308" spans="1:9">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" s="2" t="s">
         <v>0</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>238</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>2</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="311" spans="1:9">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>14</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="312" spans="1:9">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>1</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="313" spans="1:9">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>8</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:9">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>4</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:9">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>239</v>
       </c>
@@ -6133,12 +6133,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="316" spans="1:9">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="317" spans="1:9">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
         <v>7</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="318" spans="1:9">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" t="str">
         <f>B308</f>
         <v>CMP slurry production</v>
@@ -6194,7 +6194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:9">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" s="9" t="s">
         <v>156</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="320" spans="1:9">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" s="9" t="s">
         <v>162</v>
       </c>
@@ -6244,7 +6244,7 @@
       </c>
       <c r="I320" s="9"/>
     </row>
-    <row r="321" spans="1:9">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>101</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="322" spans="1:9">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" s="9"/>
       <c r="B322" s="9"/>
       <c r="C322" s="13"/>
@@ -6278,7 +6278,7 @@
       <c r="H322" s="13"/>
       <c r="I322" s="9"/>
     </row>
-    <row r="323" spans="1:9">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
         <v>0</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="324" spans="1:9">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>238</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="325" spans="1:9">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>2</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="326" spans="1:9">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>14</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="327" spans="1:9">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>1</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="328" spans="1:9">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>8</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:9">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>4</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>239</v>
       </c>
@@ -6342,12 +6342,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="332" spans="1:9">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
         <v>7</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" t="str">
         <f>B323</f>
         <v>GaAs wafer production - cleaning, quality control, packing</v>
@@ -6403,7 +6403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:9">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A334" s="9" t="s">
         <v>257</v>
       </c>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="I334" s="9"/>
     </row>
-    <row r="335" spans="1:9">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A335" s="9" t="s">
         <v>162</v>
       </c>
@@ -6451,7 +6451,7 @@
       </c>
       <c r="I335" s="9"/>
     </row>
-    <row r="336" spans="1:9">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>101</v>
       </c>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="I336" s="9"/>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A337" s="9" t="s">
         <v>176</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="338" spans="1:9">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A338" s="9" t="s">
         <v>180</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="339" spans="1:9">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A339" s="9" t="s">
         <v>183</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="340" spans="1:9">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>120</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="341" spans="1:9">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>120</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A343" s="2" t="s">
         <v>0</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>238</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>2</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>14</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>1</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>8</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:9">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>4</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="350" spans="1:9">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>239</v>
       </c>
@@ -6669,12 +6669,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="351" spans="1:9">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A352" s="2" t="s">
         <v>7</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="353" spans="1:9">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A353" t="str">
         <f>B343</f>
         <v>trimethyl aluminum 99% pure production</v>
@@ -6729,7 +6729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="354" spans="1:9">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A354" s="8" t="s">
         <v>261</v>
       </c>
@@ -6753,7 +6753,7 @@
       </c>
       <c r="I354" s="9"/>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A355" s="8" t="s">
         <v>270</v>
       </c>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="I355" s="9"/>
     </row>
-    <row r="356" spans="1:9">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A356" s="22" t="s">
         <v>269</v>
       </c>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="I356" s="9"/>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A357" s="8" t="s">
         <v>267</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="358" spans="1:9">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>120</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="359" spans="1:9">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>89</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="361" spans="1:9">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A361" s="2" t="s">
         <v>0</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="362" spans="1:9">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>238</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="363" spans="1:9">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>2</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="364" spans="1:9">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>14</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="365" spans="1:9">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>1</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="366" spans="1:9">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>8</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:9">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>4</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>239</v>
       </c>
@@ -6937,12 +6937,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="369" spans="1:9">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A369" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="370" spans="1:9">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A370" s="2" t="s">
         <v>7</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="371" spans="1:9">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A371" t="str">
         <f>B361</f>
         <v>methyl aluminum sesquichloride production</v>
@@ -6997,7 +6997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="1:9" s="25" customFormat="1">
+    <row r="372" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A372" s="22" t="s">
         <v>185</v>
       </c>
@@ -7022,7 +7022,7 @@
       <c r="H372"/>
       <c r="I372" s="22"/>
     </row>
-    <row r="373" spans="1:9">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A373" s="22" t="s">
         <v>188</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="374" spans="1:9">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A374" s="22" t="s">
         <v>189</v>
       </c>
@@ -7072,7 +7072,7 @@
       </c>
       <c r="I374" s="22"/>
     </row>
-    <row r="375" spans="1:9">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>120</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="376" spans="1:9" s="6" customFormat="1">
+    <row r="376" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376" s="22" t="s">
         <v>207</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A377" s="22" t="s">
         <v>208</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="379" spans="1:9">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A379" s="2" t="s">
         <v>0</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="380" spans="1:9">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>238</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="381" spans="1:9">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>2</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="382" spans="1:9">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>14</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="383" spans="1:9">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>1</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="384" spans="1:9">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>8</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:9">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>4</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:9">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>239</v>
       </c>
@@ -7205,12 +7205,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="387" spans="1:9">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A387" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="388" spans="1:9">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A388" s="2" t="s">
         <v>7</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="389" spans="1:9">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A389" t="str">
         <f>B379</f>
         <v>trimethyl gallium 99% pure production</v>
@@ -7265,7 +7265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="390" spans="1:9">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A390" s="22" t="s">
         <v>263</v>
       </c>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="I390" s="22"/>
     </row>
-    <row r="391" spans="1:9">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A391" s="22" t="s">
         <v>260</v>
       </c>
@@ -7313,7 +7313,7 @@
       </c>
       <c r="I391" s="22"/>
     </row>
-    <row r="392" spans="1:9">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A392" s="22" t="s">
         <v>200</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="393" spans="1:9">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>120</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="394" spans="1:9" s="6" customFormat="1">
+    <row r="394" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A394" s="22" t="s">
         <v>194</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="396" spans="1:9">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A396" s="2" t="s">
         <v>0</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="397" spans="1:9">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>238</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="398" spans="1:9">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>2</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="399" spans="1:9">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>14</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="400" spans="1:9">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>1</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="401" spans="1:9">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>8</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:9">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>4</v>
       </c>
@@ -7445,7 +7445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="403" spans="1:9">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>239</v>
       </c>
@@ -7453,12 +7453,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="404" spans="1:9">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A404" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="405" spans="1:9">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A405" s="2" t="s">
         <v>7</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="406" spans="1:9">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A406" t="str">
         <f>B396</f>
         <v>gallium chloride production</v>
@@ -7513,7 +7513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="407" spans="1:9">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A407" s="8" t="s">
         <v>129</v>
       </c>
@@ -7537,7 +7537,7 @@
       </c>
       <c r="I407" s="9"/>
     </row>
-    <row r="408" spans="1:9">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A408" s="8" t="s">
         <v>197</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="409" spans="1:9">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>120</v>
       </c>
@@ -7587,14 +7587,14 @@
       </c>
       <c r="I409" s="9"/>
     </row>
-    <row r="410" spans="1:9">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A410" s="8"/>
       <c r="B410" s="8"/>
       <c r="C410" s="21"/>
       <c r="D410" s="26"/>
       <c r="E410" s="8"/>
     </row>
-    <row r="411" spans="1:9">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A411" s="2" t="s">
         <v>0</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="412" spans="1:9">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>238</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="413" spans="1:9">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>2</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="414" spans="1:9">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>14</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="415" spans="1:9">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>1</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="416" spans="1:9">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>8</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:9">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>4</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:9">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>239</v>
       </c>
@@ -7658,12 +7658,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="419" spans="1:9">
+    <row r="419" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A419" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="420" spans="1:9">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A420" s="2" t="s">
         <v>7</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="421" spans="1:9">
+    <row r="421" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A421" t="str">
         <f>B411</f>
         <v>photovoltaic installation, 0.28kWp, GaAs</v>
@@ -7722,7 +7722,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="422" spans="1:9">
+    <row r="422" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>120</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="423" spans="1:9">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A423" s="8" t="s">
         <v>223</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>229</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="425" spans="1:9">
+    <row r="425" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>225</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="426" spans="1:9">
+    <row r="426" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A426" s="8" t="s">
         <v>243</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="427" spans="1:9">
+    <row r="427" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>282</v>
       </c>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="I427" s="28"/>
     </row>
-    <row r="429" spans="1:9">
+    <row r="429" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A429" s="2" t="s">
         <v>0</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="430" spans="1:9">
+    <row r="430" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>238</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="431" spans="1:9">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>2</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="432" spans="1:9">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>14</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="433" spans="1:13">
+    <row r="433" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>1</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="434" spans="1:13">
+    <row r="434" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>8</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:13">
+    <row r="435" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>4</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="436" spans="1:13">
+    <row r="436" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>239</v>
       </c>
@@ -7939,12 +7939,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="437" spans="1:13">
+    <row r="437" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A437" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="438" spans="1:13">
+    <row r="438" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A438" s="2" t="s">
         <v>7</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="439" spans="1:13">
+    <row r="439" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A439" t="str">
         <f>B429</f>
         <v xml:space="preserve">electricity production, photovoltaic, 0.28kWp, GaAs </v>
@@ -8011,7 +8011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="440" spans="1:13">
+    <row r="440" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A440" s="8" t="s">
         <v>272</v>
       </c>
@@ -8045,15 +8045,15 @@
         <v>8.2385895534684459E-5</v>
       </c>
       <c r="L440">
-        <f>1/0.28/1700/40/0.85/100</f>
-        <v>6.1789421651013346E-7</v>
-      </c>
-      <c r="M440">
-        <f>1/0.28/1700/20/0.85/100</f>
-        <v>1.2357884330202669E-6</v>
-      </c>
-    </row>
-    <row r="441" spans="1:13">
+        <f>1/0.28/1700/40/0.85</f>
+        <v>6.1789421651013341E-5</v>
+      </c>
+      <c r="M440" s="7">
+        <f>1/0.28/1700/20/0.85</f>
+        <v>1.2357884330202668E-4</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A441" s="28" t="s">
         <v>235</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="442" spans="1:13">
+    <row r="442" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A442" s="30" t="s">
         <v>236</v>
       </c>
@@ -8107,7 +8107,7 @@
       <c r="H442" s="28"/>
       <c r="I442" s="32"/>
     </row>
-    <row r="443" spans="1:13">
+    <row r="443" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A443" s="28" t="s">
         <v>202</v>
       </c>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="I443" s="28"/>
     </row>
-    <row r="444" spans="1:13">
+    <row r="444" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A444" s="30" t="s">
         <v>230</v>
       </c>

</xml_diff>